<commit_message>
interpolation added, added all futures
</commit_message>
<xml_diff>
--- a/data/manual/bbg_data_v2.xlsx
+++ b/data/manual/bbg_data_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlecZZX/Desktop/DS_project/data/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8ADB91-8A10-6E42-B078-63067FAFB5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A2CFD6-D425-194B-874F-D3451680CBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9116,10 +9116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D434"/>
+  <dimension ref="A1:D406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
-      <selection activeCell="H413" sqref="H413"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14812,398 +14812,6 @@
         <v>4297.75</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A407" s="1">
-        <v>44498</v>
-      </c>
-      <c r="B407">
-        <v>1.2962</v>
-      </c>
-      <c r="C407">
-        <v>4605.38</v>
-      </c>
-      <c r="D407">
-        <v>4597</v>
-      </c>
-    </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A408" s="1">
-        <v>44530</v>
-      </c>
-      <c r="B408">
-        <v>1.3221000000000001</v>
-      </c>
-      <c r="C408">
-        <v>4567</v>
-      </c>
-      <c r="D408">
-        <v>4566.25</v>
-      </c>
-    </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A409" s="1">
-        <v>44561</v>
-      </c>
-      <c r="B409">
-        <v>1.2701</v>
-      </c>
-      <c r="C409">
-        <v>4766.18</v>
-      </c>
-      <c r="D409">
-        <v>4758.5</v>
-      </c>
-    </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A410" s="1">
-        <v>44592</v>
-      </c>
-      <c r="B410">
-        <v>1.3443000000000001</v>
-      </c>
-      <c r="C410">
-        <v>4515.55</v>
-      </c>
-      <c r="D410">
-        <v>4504.25</v>
-      </c>
-    </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A411" s="1">
-        <v>44620</v>
-      </c>
-      <c r="B411">
-        <v>1.4048</v>
-      </c>
-      <c r="C411">
-        <v>4373.9399999999996</v>
-      </c>
-      <c r="D411">
-        <v>4368</v>
-      </c>
-    </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A412" s="1">
-        <v>44651</v>
-      </c>
-      <c r="B412">
-        <v>1.3714</v>
-      </c>
-      <c r="C412">
-        <v>4530.41</v>
-      </c>
-      <c r="D412">
-        <v>4530.75</v>
-      </c>
-    </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A413" s="1">
-        <v>44680</v>
-      </c>
-      <c r="B413">
-        <v>1.5084</v>
-      </c>
-      <c r="C413">
-        <v>4131.93</v>
-      </c>
-      <c r="D413">
-        <v>4127.5</v>
-      </c>
-    </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A414" s="1">
-        <v>44712</v>
-      </c>
-      <c r="B414">
-        <v>1.5305</v>
-      </c>
-      <c r="C414">
-        <v>4132.1499999999996</v>
-      </c>
-      <c r="D414">
-        <v>4131.25</v>
-      </c>
-    </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A415" s="1">
-        <v>44742</v>
-      </c>
-      <c r="B415">
-        <v>1.6974</v>
-      </c>
-      <c r="C415">
-        <v>3785.38</v>
-      </c>
-      <c r="D415">
-        <v>3789.5</v>
-      </c>
-    </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A416" s="1">
-        <v>44771</v>
-      </c>
-      <c r="B416">
-        <v>1.5620000000000001</v>
-      </c>
-      <c r="C416">
-        <v>4130.29</v>
-      </c>
-      <c r="D416">
-        <v>4133.5</v>
-      </c>
-    </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A417" s="1">
-        <v>44804</v>
-      </c>
-      <c r="B417">
-        <v>1.6534</v>
-      </c>
-      <c r="C417">
-        <v>3955</v>
-      </c>
-      <c r="D417">
-        <v>3956.5</v>
-      </c>
-    </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A418" s="1">
-        <v>44834</v>
-      </c>
-      <c r="B418">
-        <v>1.8493999999999999</v>
-      </c>
-      <c r="C418">
-        <v>3585.62</v>
-      </c>
-      <c r="D418">
-        <v>3601.5</v>
-      </c>
-    </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A419" s="1">
-        <v>44865</v>
-      </c>
-      <c r="B419">
-        <v>1.7118</v>
-      </c>
-      <c r="C419">
-        <v>3871.98</v>
-      </c>
-      <c r="D419">
-        <v>3883</v>
-      </c>
-    </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A420" s="1">
-        <v>44895</v>
-      </c>
-      <c r="B420">
-        <v>1.6437999999999999</v>
-      </c>
-      <c r="C420">
-        <v>4080.11</v>
-      </c>
-      <c r="D420">
-        <v>4081.25</v>
-      </c>
-    </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A421" s="1">
-        <v>44925</v>
-      </c>
-      <c r="B421">
-        <v>1.7599</v>
-      </c>
-      <c r="C421">
-        <v>3839.5</v>
-      </c>
-      <c r="D421">
-        <v>3861</v>
-      </c>
-    </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A422" s="1">
-        <v>44957</v>
-      </c>
-      <c r="B422">
-        <v>1.6576</v>
-      </c>
-      <c r="C422">
-        <v>4076.6</v>
-      </c>
-      <c r="D422">
-        <v>4090</v>
-      </c>
-    </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A423" s="1">
-        <v>44985</v>
-      </c>
-      <c r="B423">
-        <v>1.7225999999999999</v>
-      </c>
-      <c r="C423">
-        <v>3970.15</v>
-      </c>
-      <c r="D423">
-        <v>3975.5</v>
-      </c>
-    </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A424" s="1">
-        <v>45016</v>
-      </c>
-      <c r="B424">
-        <v>1.6758999999999999</v>
-      </c>
-      <c r="C424">
-        <v>4109.3100000000004</v>
-      </c>
-      <c r="D424">
-        <v>4137.75</v>
-      </c>
-    </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A425" s="1">
-        <v>45044</v>
-      </c>
-      <c r="B425">
-        <v>1.6574</v>
-      </c>
-      <c r="C425">
-        <v>4169.4799999999996</v>
-      </c>
-      <c r="D425">
-        <v>4188.5</v>
-      </c>
-    </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A426" s="1">
-        <v>45077</v>
-      </c>
-      <c r="B426">
-        <v>1.6569</v>
-      </c>
-      <c r="C426">
-        <v>4179.83</v>
-      </c>
-      <c r="D426">
-        <v>4190.5</v>
-      </c>
-    </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A427" s="1">
-        <v>45107</v>
-      </c>
-      <c r="B427">
-        <v>1.5535000000000001</v>
-      </c>
-      <c r="C427">
-        <v>4450.38</v>
-      </c>
-      <c r="D427">
-        <v>4488.25</v>
-      </c>
-    </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A428" s="1">
-        <v>45138</v>
-      </c>
-      <c r="B428">
-        <v>1.5065999999999999</v>
-      </c>
-      <c r="C428">
-        <v>4588.96</v>
-      </c>
-      <c r="D428">
-        <v>4614.5</v>
-      </c>
-    </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A429" s="1">
-        <v>45169</v>
-      </c>
-      <c r="B429">
-        <v>1.5384</v>
-      </c>
-      <c r="C429">
-        <v>4507.66</v>
-      </c>
-      <c r="D429">
-        <v>4516</v>
-      </c>
-    </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A430" s="1">
-        <v>45198</v>
-      </c>
-      <c r="B430">
-        <v>1.6111</v>
-      </c>
-      <c r="C430">
-        <v>4288.05</v>
-      </c>
-      <c r="D430">
-        <v>4325.5</v>
-      </c>
-    </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A431" s="1">
-        <v>45230</v>
-      </c>
-      <c r="B431">
-        <v>1.6512</v>
-      </c>
-      <c r="C431">
-        <v>4193.8</v>
-      </c>
-      <c r="D431">
-        <v>4212.25</v>
-      </c>
-    </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A432" s="1">
-        <v>45260</v>
-      </c>
-      <c r="B432">
-        <v>1.5322</v>
-      </c>
-      <c r="C432">
-        <v>4567.8</v>
-      </c>
-      <c r="D432">
-        <v>4576.75</v>
-      </c>
-    </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A433" s="1">
-        <v>45289</v>
-      </c>
-      <c r="B433">
-        <v>1.4865999999999999</v>
-      </c>
-      <c r="C433">
-        <v>4769.83</v>
-      </c>
-      <c r="D433">
-        <v>4820</v>
-      </c>
-    </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A434" s="1">
-        <v>45322</v>
-      </c>
-      <c r="B434">
-        <v>1.4695</v>
-      </c>
-      <c r="C434">
-        <v>4845.6499999999996</v>
-      </c>
-      <c r="D434">
-        <v>4870.5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>